<commit_message>
officially add bwaise systems to package; add test function
</commit_message>
<xml_diff>
--- a/qsdsan/systems/bwaise/results/sysC.xlsx
+++ b/qsdsan/systems/bwaise/results/sysC.xlsx
@@ -8,68 +8,166 @@
   </bookViews>
   <sheets>
     <sheet name="Flowsheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Stream table" sheetId="2" r:id="rId2"/>
-    <sheet name="Utilities" sheetId="3" r:id="rId3"/>
-    <sheet name="Design requirements" sheetId="4" r:id="rId4"/>
+    <sheet name="Itemized costs" sheetId="2" r:id="rId2"/>
+    <sheet name="Cash flow" sheetId="3" r:id="rId3"/>
+    <sheet name="Stream table" sheetId="4" r:id="rId4"/>
+    <sheet name="Utilities" sheetId="5" r:id="rId5"/>
+    <sheet name="Design requirements" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="154">
+  <si>
+    <t>Unit operation</t>
+  </si>
+  <si>
+    <t>Purchase cost (10^6 USD)</t>
+  </si>
+  <si>
+    <t>Utility cost (10^6 USD/yr)</t>
+  </si>
+  <si>
+    <t>Installed cost (10^6 USD)</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>Anaerobic lagoon</t>
+  </si>
+  <si>
+    <t>Facultative lagoon</t>
+  </si>
+  <si>
+    <t>Trucking</t>
+  </si>
+  <si>
+    <t>UDDT</t>
+  </si>
+  <si>
+    <t>Unplanted drying bed</t>
+  </si>
+  <si>
+    <t>Depreciable capital [MM$]</t>
+  </si>
+  <si>
+    <t>Fixed capital investment [MM$]</t>
+  </si>
+  <si>
+    <t>Working capital [MM$]</t>
+  </si>
+  <si>
+    <t>Depreciation [MM$]</t>
+  </si>
+  <si>
+    <t>Loan [MM$]</t>
+  </si>
+  <si>
+    <t>Loan interest payment [MM$]</t>
+  </si>
+  <si>
+    <t>Loan payment [MM$]</t>
+  </si>
+  <si>
+    <t>Loan principal [MM$]</t>
+  </si>
+  <si>
+    <t>Annual operating cost (excluding depreciation) [MM$]</t>
+  </si>
+  <si>
+    <t>Sales [MM$]</t>
+  </si>
+  <si>
+    <t>Tax [MM$]</t>
+  </si>
+  <si>
+    <t>Incentives [MM$]</t>
+  </si>
+  <si>
+    <t>Net earnings [MM$]</t>
+  </si>
+  <si>
+    <t>Cash flow [MM$]</t>
+  </si>
+  <si>
+    <t>Discount factor</t>
+  </si>
+  <si>
+    <t>Net present value (NPV) [MM$]</t>
+  </si>
+  <si>
+    <t>Cumulative NPV [MM$]</t>
+  </si>
   <si>
     <t>toilet_paper</t>
   </si>
   <si>
+    <t>reuse_loss</t>
+  </si>
+  <si>
+    <t>evaporated</t>
+  </si>
+  <si>
     <t>C2_N2O</t>
   </si>
   <si>
     <t>sol_waste</t>
   </si>
   <si>
+    <t>C_liq_K</t>
+  </si>
+  <si>
+    <t>ws3</t>
+  </si>
+  <si>
     <t>C6_N2O</t>
   </si>
   <si>
-    <t>ws5</t>
-  </si>
-  <si>
-    <t>reuse_loss</t>
-  </si>
-  <si>
-    <t>evaporated</t>
-  </si>
-  <si>
-    <t>C_liq_K</t>
-  </si>
-  <si>
     <t>C_N2O</t>
   </si>
   <si>
+    <t>C_sol_non_fertilizers</t>
+  </si>
+  <si>
     <t>transported_l</t>
   </si>
   <si>
+    <t>C_sol_K</t>
+  </si>
+  <si>
+    <t>C8_CH4</t>
+  </si>
+  <si>
+    <t>struvite</t>
+  </si>
+  <si>
+    <t>ws4</t>
+  </si>
+  <si>
     <t>facultative_treated</t>
   </si>
   <si>
-    <t>ws6</t>
-  </si>
-  <si>
-    <t>struvite</t>
-  </si>
-  <si>
-    <t>C8_CH4</t>
-  </si>
-  <si>
-    <t>C_sol_K</t>
-  </si>
-  <si>
     <t>C_liq_N</t>
   </si>
   <si>
-    <t>C_sol_non_fertilizers</t>
-  </si>
-  <si>
     <t>flushing_water</t>
   </si>
   <si>
@@ -79,52 +177,58 @@
     <t>C7_CH4</t>
   </si>
   <si>
+    <t>C_sol_N</t>
+  </si>
+  <si>
     <t>urine</t>
   </si>
   <si>
     <t>HAP</t>
   </si>
   <si>
+    <t>C8_N2O</t>
+  </si>
+  <si>
+    <t>C_liq_non_fertilizers</t>
+  </si>
+  <si>
     <t>anaerobic_treated</t>
   </si>
   <si>
-    <t>C8_N2O</t>
-  </si>
-  <si>
-    <t>C_sol_N</t>
-  </si>
-  <si>
-    <t>C_liq_non_fertilizers</t>
-  </si>
-  <si>
     <t>loss_l</t>
   </si>
   <si>
+    <t>desiccant</t>
+  </si>
+  <si>
+    <t>C_liq_P</t>
+  </si>
+  <si>
+    <t>liquid_fertilizer</t>
+  </si>
+  <si>
+    <t>C2_CH4</t>
+  </si>
+  <si>
+    <t>C6_CH4</t>
+  </si>
+  <si>
+    <t>C_CH4</t>
+  </si>
+  <si>
+    <t>feces</t>
+  </si>
+  <si>
     <t>transported_s</t>
   </si>
   <si>
-    <t>desiccant</t>
-  </si>
-  <si>
-    <t>C6_CH4</t>
-  </si>
-  <si>
-    <t>feces</t>
-  </si>
-  <si>
-    <t>C2_CH4</t>
-  </si>
-  <si>
     <t>C7_N2O</t>
   </si>
   <si>
-    <t>liquid_fertilizer</t>
-  </si>
-  <si>
-    <t>C_CH4</t>
-  </si>
-  <si>
-    <t>C_liq_P</t>
+    <t>dried_sludge</t>
+  </si>
+  <si>
+    <t>C_sol_P</t>
   </si>
   <si>
     <t>liq_waste</t>
@@ -133,12 +237,6 @@
     <t>loss_s</t>
   </si>
   <si>
-    <t>dried_sludge</t>
-  </si>
-  <si>
-    <t>C_sol_P</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -211,51 +309,33 @@
     <t>-</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>liquid</t>
   </si>
   <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
     <t>C11</t>
   </si>
   <si>
-    <t>gas</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C6</t>
+    <t>C13</t>
   </si>
   <si>
     <t>C5</t>
   </si>
   <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C7</t>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C10</t>
   </si>
   <si>
     <t>solid</t>
   </si>
   <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -274,9 +354,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>Anaerobic lagoon</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
@@ -316,18 +393,9 @@
     <t>USD/hr</t>
   </si>
   <si>
-    <t>Facultative lagoon</t>
-  </si>
-  <si>
-    <t>Trucking</t>
-  </si>
-  <si>
     <t>Parallel trucks</t>
   </si>
   <si>
-    <t>UDDT</t>
-  </si>
-  <si>
     <t>Purchase cost</t>
   </si>
   <si>
@@ -380,9 +448,6 @@
   </si>
   <si>
     <t>USD</t>
-  </si>
-  <si>
-    <t>Unplanted drying bed</t>
   </si>
   <si>
     <t>Number of covered bed</t>
@@ -829,6 +894,705 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>15.7835531875</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>15.7835531875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B2">
+        <v>15.7835531875</v>
+      </c>
+      <c r="C2">
+        <v>15.7835531875</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>-15.7835531875</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>-15.7835531875</v>
+      </c>
+      <c r="R2">
+        <v>-15.7835531875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2.25546975049375</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K3">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>-14.43911035832047</v>
+      </c>
+      <c r="O3">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P3">
+        <v>0.9523809523809523</v>
+      </c>
+      <c r="Q3">
+        <v>-11.60346724554925</v>
+      </c>
+      <c r="R3">
+        <v>-27.38702043304925</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3.86539217561875</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K4">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>-16.04903278344547</v>
+      </c>
+      <c r="O4">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P4">
+        <v>0.9070294784580498</v>
+      </c>
+      <c r="Q4">
+        <v>-11.05092118623738</v>
+      </c>
+      <c r="R4">
+        <v>-38.43794161928664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>2.76054345249375</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K5">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>-14.94418406032046</v>
+      </c>
+      <c r="O5">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P5">
+        <v>0.863837598531476</v>
+      </c>
+      <c r="Q5">
+        <v>-10.5246868440356</v>
+      </c>
+      <c r="R5">
+        <v>-48.96262846332225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1.97136579311875</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K6">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>-14.15500640094547</v>
+      </c>
+      <c r="O6">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P6">
+        <v>0.8227024747918819</v>
+      </c>
+      <c r="Q6">
+        <v>-10.02351128003391</v>
+      </c>
+      <c r="R6">
+        <v>-58.98613974335615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1.40947129964375</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K7">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>-13.59311190747047</v>
+      </c>
+      <c r="O7">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P7">
+        <v>0.7835261664684589</v>
+      </c>
+      <c r="Q7">
+        <v>-9.54620121907991</v>
+      </c>
+      <c r="R7">
+        <v>-68.53234096243607</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1.407892944325</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K8">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>-13.59153355215171</v>
+      </c>
+      <c r="O8">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P8">
+        <v>0.7462153966366274</v>
+      </c>
+      <c r="Q8">
+        <v>-9.091620208647532</v>
+      </c>
+      <c r="R8">
+        <v>-77.62396117108359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1.40947129964375</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K9">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>-13.59311190747047</v>
+      </c>
+      <c r="O9">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P9">
+        <v>0.7106813301301214</v>
+      </c>
+      <c r="Q9">
+        <v>-8.658685912997649</v>
+      </c>
+      <c r="R9">
+        <v>-86.28264708408125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-0</v>
+      </c>
+      <c r="E10">
+        <v>0.7039464721625001</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>12.72357373677861</v>
+      </c>
+      <c r="K10">
+        <v>0.5399331289518972</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>-12.88758707998922</v>
+      </c>
+      <c r="O10">
+        <v>-12.18364060782672</v>
+      </c>
+      <c r="P10">
+        <v>0.676839362028687</v>
+      </c>
+      <c r="Q10">
+        <v>-8.246367536188238</v>
+      </c>
+      <c r="R10">
+        <v>-94.52901462026949</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AO26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -837,504 +1601,504 @@
   <sheetData>
     <row r="2" spans="1:41">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:41">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="P3" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="Q3" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="R3" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="S3" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="T3" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="U3" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="V3" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="W3" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="X3" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="Y3" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="Z3" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="AA3" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="AB3" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="AC3" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="AD3" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="AE3" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="AF3" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="AG3" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="AH3" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="AI3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="AJ3" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="AK3" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="AL3" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="AM3" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="AN3" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="AO3" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:41">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="K4" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="L4" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="M4" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="N4" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="O4" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="P4" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="Q4" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="R4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="S4" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="T4" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="U4" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="V4" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="W4" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="X4" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="Y4" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="Z4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="AA4" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="AB4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="AC4" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="AD4" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="AE4" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="AF4" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AG4" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="AH4" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="AI4" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="AJ4" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="AK4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="AL4" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="AM4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="AN4" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="AO4" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:41">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="N5" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="O5" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="P5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="Q5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="R5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="S5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="T5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="U5" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="V5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="W5" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="X5" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="Y5" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="Z5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AA5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AB5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AC5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AD5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AE5" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="AF5" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="AG5" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="AH5" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="AI5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AJ5" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="AK5" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="AL5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AM5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AN5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AO5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:41">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>298.15</v>
@@ -1459,58 +2223,58 @@
     </row>
     <row r="7" spans="1:41">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>0.000281583</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>4.921641701924244</v>
       </c>
       <c r="D7">
+        <v>97328.93178550167</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>113011.4206765087</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="G7">
+        <v>30.41695816694304</v>
+      </c>
+      <c r="H7">
         <v>26092.86888254258</v>
       </c>
-      <c r="G7">
-        <v>4.921641701924244</v>
-      </c>
-      <c r="H7">
-        <v>97328.93178550167</v>
-      </c>
       <c r="I7">
-        <v>30.41695816694304</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0.3912074638652792</v>
       </c>
       <c r="K7">
+        <v>13163.80440493071</v>
+      </c>
+      <c r="L7">
         <v>26092.86888254258</v>
       </c>
-      <c r="L7">
+      <c r="M7">
+        <v>10.905142199952</v>
+      </c>
+      <c r="N7">
+        <v>10.37468720194036</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>110751.1922629785</v>
+      </c>
+      <c r="Q7">
         <v>25035.15925874464</v>
       </c>
-      <c r="M7">
-        <v>110751.1922629785</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>10.37468720194036</v>
-      </c>
-      <c r="P7">
-        <v>10.905142199952</v>
-      </c>
-      <c r="Q7">
+      <c r="R7">
         <v>89.0136458913077</v>
-      </c>
-      <c r="R7">
-        <v>13163.80440493071</v>
       </c>
       <c r="S7">
         <v>0.4166666669999999</v>
@@ -1522,96 +2286,96 @@
         <v>0.9931671354828903</v>
       </c>
       <c r="V7">
+        <v>8.834627801783146</v>
+      </c>
+      <c r="W7">
         <v>0.05833333333333333</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>13.35498580967109</v>
-      </c>
-      <c r="X7">
-        <v>25293.95457086856</v>
       </c>
       <c r="Y7">
         <v>0.04941379251340257</v>
       </c>
       <c r="Z7">
-        <v>8.834627801783146</v>
+        <v>24907.19607091476</v>
       </c>
       <c r="AA7">
-        <v>24907.19607091476</v>
+        <v>25293.95457086856</v>
       </c>
       <c r="AB7">
         <v>532.5075282151539</v>
       </c>
       <c r="AC7">
+        <v>0.0063308</v>
+      </c>
+      <c r="AD7">
+        <v>3.610942069701285</v>
+      </c>
+      <c r="AE7">
+        <v>25030.23761704271</v>
+      </c>
+      <c r="AF7">
+        <v>0.1687239654291444</v>
+      </c>
+      <c r="AG7">
+        <v>13.2422284731052</v>
+      </c>
+      <c r="AH7">
+        <v>24.7788067759576</v>
+      </c>
+      <c r="AI7">
+        <v>0.01041666666666667</v>
+      </c>
+      <c r="AJ7">
         <v>110751.1922629785</v>
       </c>
-      <c r="AD7">
-        <v>0.0063308</v>
-      </c>
-      <c r="AE7">
-        <v>13.2422284731052</v>
-      </c>
-      <c r="AF7">
-        <v>0.01041666666666667</v>
-      </c>
-      <c r="AG7">
-        <v>0.1687239654291444</v>
-      </c>
-      <c r="AH7">
+      <c r="AK7">
         <v>0.3417936713518766</v>
       </c>
-      <c r="AI7">
-        <v>25030.23761704271</v>
-      </c>
-      <c r="AJ7">
-        <v>24.7788067759576</v>
-      </c>
-      <c r="AK7">
-        <v>3.610942069701285</v>
-      </c>
       <c r="AL7">
+        <v>13190.98146271362</v>
+      </c>
+      <c r="AM7">
+        <v>7.437287781173251</v>
+      </c>
+      <c r="AN7">
         <v>26625.37641075773</v>
       </c>
-      <c r="AM7">
+      <c r="AO7">
         <v>2260.228413530177</v>
-      </c>
-      <c r="AN7">
-        <v>13190.98146271362</v>
-      </c>
-      <c r="AO7">
-        <v>7.437287781173251</v>
       </c>
     </row>
     <row r="8" spans="1:41">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:41">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>77.524293704849</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>0.002586065046122275</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>0.3445517096679769</v>
       </c>
-      <c r="G9">
-        <v>77.524293704849</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
         <v>0</v>
       </c>
@@ -1619,29 +2383,29 @@
         <v>0</v>
       </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>0.3445517096679769</v>
       </c>
-      <c r="L9">
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0.002586065046122275</v>
+      </c>
+      <c r="Q9">
         <v>0.3048087634407487</v>
       </c>
-      <c r="M9">
-        <v>0.002586065046122275</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
+      <c r="R9">
         <v>81.44132359483623</v>
       </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
       <c r="S9">
         <v>0</v>
       </c>
@@ -1652,91 +2416,91 @@
         <v>0</v>
       </c>
       <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
         <v>0.3659002285714285</v>
       </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
       <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
         <v>0.3554344402111291</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
       </c>
       <c r="AB9">
         <v>0.344551709667977</v>
       </c>
       <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0.2896252624647141</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0.06574463999999999</v>
+      </c>
+      <c r="AJ9">
         <v>0.002586065046122275</v>
       </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AF9">
-        <v>0.06574463999999999</v>
-      </c>
-      <c r="AG9">
-        <v>0</v>
-      </c>
-      <c r="AH9">
-        <v>0</v>
-      </c>
-      <c r="AI9">
-        <v>0.2896252624647141</v>
-      </c>
-      <c r="AJ9">
-        <v>0</v>
-      </c>
       <c r="AK9">
         <v>0</v>
       </c>
       <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
         <v>0.344551709667977</v>
       </c>
-      <c r="AM9">
+      <c r="AO9">
         <v>0.00258606504612227</v>
-      </c>
-      <c r="AN9">
-        <v>0</v>
-      </c>
-      <c r="AO9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:41">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>6.850109522479641</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>0.0110694592248413</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>0.06460344556274569</v>
       </c>
-      <c r="G10">
-        <v>6.850109522479641</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
         <v>0</v>
       </c>
@@ -1744,29 +2508,29 @@
         <v>0</v>
       </c>
       <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>0.06460344556274569</v>
       </c>
-      <c r="L10">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0.0110694592248413</v>
+      </c>
+      <c r="Q10">
         <v>0.06733287441901928</v>
       </c>
-      <c r="M10">
-        <v>0.0110694592248413</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
+      <c r="R10">
         <v>18.55867640516378</v>
       </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
       <c r="S10">
         <v>0</v>
       </c>
@@ -1777,91 +2541,91 @@
         <v>0</v>
       </c>
       <c r="V10">
+        <v>100</v>
+      </c>
+      <c r="W10">
         <v>0.06457062857142859</v>
       </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
       <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
         <v>0.06664395753958674</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <v>100</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
       </c>
       <c r="AB10">
         <v>0.06460344556274587</v>
       </c>
       <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0.06599919165832493</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0.26297856</v>
+      </c>
+      <c r="AJ10">
         <v>0.0110694592248413</v>
       </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <v>0.26297856</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <v>0.06599919165832493</v>
-      </c>
-      <c r="AJ10">
-        <v>0</v>
-      </c>
       <c r="AK10">
         <v>0</v>
       </c>
       <c r="AL10">
+        <v>0.06697475716083454</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
         <v>0.06460344556274571</v>
       </c>
-      <c r="AM10">
+      <c r="AO10">
         <v>0.01106945922484128</v>
-      </c>
-      <c r="AN10">
-        <v>0.06697475716083454</v>
-      </c>
-      <c r="AO10">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:41">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.497319385749154</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>0.006715311708350213</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>0.03530308205651655</v>
       </c>
-      <c r="G11">
-        <v>1.497319385749154</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
       <c r="I11">
         <v>0</v>
       </c>
@@ -1869,26 +2633,26 @@
         <v>0</v>
       </c>
       <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>0.03530308205651655</v>
       </c>
-      <c r="L11">
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0.006715311708350213</v>
+      </c>
+      <c r="Q11">
         <v>0.01471784032575822</v>
       </c>
-      <c r="M11">
-        <v>0.006715311708350213</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
       <c r="R11">
         <v>0</v>
       </c>
@@ -1902,118 +2666,118 @@
         <v>0</v>
       </c>
       <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
         <v>0.04455919285714285</v>
       </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
       <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
         <v>0.03641813654205105</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
       </c>
       <c r="AB11">
         <v>0.03530308205651645</v>
       </c>
       <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>100</v>
+      </c>
+      <c r="AE11">
+        <v>0.01442631957773605</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0.15953652</v>
+      </c>
+      <c r="AJ11">
         <v>0.006715311708350213</v>
       </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0.15953652</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>0.01442631957773605</v>
-      </c>
-      <c r="AJ11">
-        <v>0</v>
-      </c>
       <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0.05638161043737278</v>
+      </c>
+      <c r="AM11">
         <v>100</v>
       </c>
-      <c r="AL11">
+      <c r="AN11">
         <v>0.03530308205651655</v>
       </c>
-      <c r="AM11">
+      <c r="AO11">
         <v>0.006715311708350196</v>
-      </c>
-      <c r="AN11">
-        <v>0.05638161043737278</v>
-      </c>
-      <c r="AO11">
-        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:41">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>12.61274765414683</v>
       </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>0.009846523524602569</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
         <v>0.1189509384919102</v>
       </c>
-      <c r="G12">
-        <v>12.61274765414683</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.1189509384919102</v>
+      </c>
+      <c r="M12">
         <v>100</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0.1189509384919102</v>
-      </c>
-      <c r="L12">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0.009846523524602569</v>
+      </c>
+      <c r="Q12">
         <v>0.1239764927974513</v>
       </c>
-      <c r="M12">
-        <v>0.009846523524602569</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>100</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
       <c r="R12">
         <v>0</v>
       </c>
@@ -2027,91 +2791,91 @@
         <v>0</v>
       </c>
       <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
         <v>0.1188905142857143</v>
       </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
       <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
         <v>0.1227080262530186</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <v>0</v>
       </c>
       <c r="AB12">
         <v>0.1189509384919097</v>
       </c>
       <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0.1215208526275939</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0.23392512</v>
+      </c>
+      <c r="AJ12">
         <v>0.009846523524602569</v>
       </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <v>0.23392512</v>
-      </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>0</v>
-      </c>
-      <c r="AI12">
-        <v>0.1215208526275939</v>
-      </c>
-      <c r="AJ12">
-        <v>0</v>
-      </c>
       <c r="AK12">
         <v>0</v>
       </c>
       <c r="AL12">
+        <v>0.08267119645931652</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
         <v>0.1189509384919103</v>
       </c>
-      <c r="AM12">
+      <c r="AO12">
         <v>0.009846523524602566</v>
-      </c>
-      <c r="AN12">
-        <v>0.08267119645931652</v>
-      </c>
-      <c r="AO12">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:41">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1.515529732775368</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>0.004209263000315044</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>0.01429297477197631</v>
       </c>
-      <c r="G13">
-        <v>1.515529732775368</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
       <c r="I13">
         <v>0</v>
       </c>
@@ -2119,28 +2883,28 @@
         <v>0</v>
       </c>
       <c r="K13">
+        <v>0.03541384249516179</v>
+      </c>
+      <c r="L13">
         <v>0.01429297477197631</v>
       </c>
-      <c r="L13">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0.004209263000315044</v>
+      </c>
+      <c r="Q13">
         <v>0.01489683819512349</v>
       </c>
-      <c r="M13">
-        <v>0.004209263000315044</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
       <c r="R13">
-        <v>0.03541384249516179</v>
+        <v>0</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -2152,69 +2916,69 @@
         <v>0</v>
       </c>
       <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <v>0.01428571428571429</v>
       </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
       <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0.0146739047339065</v>
+      </c>
+      <c r="AA13">
         <v>0.0147444210679572</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0.0146739047339065</v>
       </c>
       <c r="AB13">
         <v>0.01429297477197634</v>
       </c>
       <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0.01460177198176016</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>0.1</v>
+      </c>
+      <c r="AJ13">
         <v>0.004209263000315044</v>
       </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AF13">
-        <v>0.1</v>
-      </c>
-      <c r="AG13">
-        <v>0</v>
-      </c>
-      <c r="AH13">
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <v>0.01460177198176016</v>
-      </c>
-      <c r="AJ13">
-        <v>0</v>
-      </c>
       <c r="AK13">
         <v>0</v>
       </c>
       <c r="AL13">
+        <v>0.03534088021812985</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
         <v>0.01429297477197631</v>
       </c>
-      <c r="AM13">
+      <c r="AO13">
         <v>0.004209263000315029</v>
-      </c>
-      <c r="AN13">
-        <v>0.03534088021812985</v>
-      </c>
-      <c r="AO13">
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:41">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2223,14 +2987,14 @@
         <v>0</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>0.03199039880239433</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
         <v>0</v>
       </c>
@@ -2244,28 +3008,28 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>0.2691452029632296</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>0.03199039880239433</v>
       </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>0.2691452029632296</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -2277,11 +3041,11 @@
         <v>0</v>
       </c>
       <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
         <v>0.02</v>
       </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
       <c r="X14">
         <v>0</v>
       </c>
@@ -2298,48 +3062,48 @@
         <v>0</v>
       </c>
       <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0.7599999999999999</v>
+      </c>
+      <c r="AJ14">
         <v>0.03199039880239433</v>
       </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-      <c r="AE14">
-        <v>0</v>
-      </c>
-      <c r="AF14">
-        <v>0.7599999999999999</v>
-      </c>
-      <c r="AG14">
-        <v>0</v>
-      </c>
-      <c r="AH14">
-        <v>0</v>
-      </c>
-      <c r="AI14">
-        <v>0</v>
-      </c>
-      <c r="AJ14">
-        <v>0</v>
-      </c>
       <c r="AK14">
         <v>0</v>
       </c>
       <c r="AL14">
-        <v>0</v>
+        <v>0.2685906896577868</v>
       </c>
       <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
         <v>0.03199039880239428</v>
-      </c>
-      <c r="AN14">
-        <v>0.2685906896577868</v>
-      </c>
-      <c r="AO14">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:41">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2348,20 +3112,20 @@
         <v>0</v>
       </c>
       <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>96.70327422839901</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>95.04828223364245</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>100</v>
-      </c>
       <c r="I15">
         <v>0</v>
       </c>
@@ -2369,28 +3133,28 @@
         <v>0</v>
       </c>
       <c r="K15">
+        <v>74.22700215849414</v>
+      </c>
+      <c r="L15">
         <v>95.04828223364245</v>
       </c>
-      <c r="L15">
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>96.70327422839901</v>
+      </c>
+      <c r="Q15">
         <v>99.06397399757124</v>
       </c>
-      <c r="M15">
-        <v>96.70327422839901</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
       <c r="R15">
-        <v>74.22700215849414</v>
+        <v>0</v>
       </c>
       <c r="S15">
         <v>100</v>
@@ -2402,69 +3166,69 @@
         <v>0</v>
       </c>
       <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
         <v>94.99999999999999</v>
       </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
       <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>99.5729249800798</v>
+      </c>
+      <c r="AA15">
         <v>98.05040010191537</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>99.5729249800798</v>
       </c>
       <c r="AB15">
         <v>95.04828223364244</v>
       </c>
       <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>99.0834527333725</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>85</v>
+      </c>
+      <c r="AJ15">
         <v>96.70327422839901</v>
       </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
-      <c r="AF15">
-        <v>85</v>
-      </c>
-      <c r="AG15">
-        <v>0</v>
-      </c>
-      <c r="AH15">
-        <v>0</v>
-      </c>
-      <c r="AI15">
-        <v>99.0834527333725</v>
-      </c>
-      <c r="AJ15">
-        <v>0</v>
-      </c>
       <c r="AK15">
         <v>0</v>
       </c>
       <c r="AL15">
+        <v>74.07407407407408</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
         <v>95.04828223364247</v>
       </c>
-      <c r="AM15">
+      <c r="AO15">
         <v>96.70327422839901</v>
-      </c>
-      <c r="AN15">
-        <v>74.07407407407408</v>
-      </c>
-      <c r="AO15">
-        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:41">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2473,20 +3237,20 @@
         <v>0</v>
       </c>
       <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>0.5583158761363954</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>4.374015615806415</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16">
         <v>0</v>
       </c>
@@ -2494,28 +3258,28 @@
         <v>0</v>
       </c>
       <c r="K16">
+        <v>2.988129348397645</v>
+      </c>
+      <c r="L16">
         <v>4.374015615806415</v>
       </c>
-      <c r="L16">
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0.5583158761363954</v>
+      </c>
+      <c r="Q16">
         <v>0.4102931932506434</v>
       </c>
-      <c r="M16">
-        <v>0.5583158761363954</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
       <c r="R16">
-        <v>2.988129348397645</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -2527,69 +3291,69 @@
         <v>0</v>
       </c>
       <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
         <v>4.371793721428576</v>
       </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
       <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0.4124011151862868</v>
+      </c>
+      <c r="AA16">
         <v>1.353650916470885</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AA16">
-        <v>0.4124011151862868</v>
       </c>
       <c r="AB16">
         <v>4.374015615806415</v>
       </c>
       <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0.4103738683173692</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>13.41781515999999</v>
+      </c>
+      <c r="AJ16">
         <v>0.5583158761363954</v>
       </c>
-      <c r="AD16">
-        <v>0</v>
-      </c>
-      <c r="AE16">
-        <v>0</v>
-      </c>
-      <c r="AF16">
-        <v>13.41781515999999</v>
-      </c>
-      <c r="AG16">
-        <v>0</v>
-      </c>
-      <c r="AH16">
-        <v>0</v>
-      </c>
-      <c r="AI16">
-        <v>0.4103738683173692</v>
-      </c>
-      <c r="AJ16">
-        <v>0</v>
-      </c>
       <c r="AK16">
         <v>0</v>
       </c>
       <c r="AL16">
+        <v>2.981972978290253</v>
+      </c>
+      <c r="AM16">
+        <v>0</v>
+      </c>
+      <c r="AN16">
         <v>4.374015615806416</v>
       </c>
-      <c r="AM16">
+      <c r="AO16">
         <v>0.5583158761363949</v>
-      </c>
-      <c r="AN16">
-        <v>2.981972978290253</v>
-      </c>
-      <c r="AO16">
-        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:41">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2688,16 +3452,16 @@
         <v>0</v>
       </c>
       <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
         <v>100</v>
-      </c>
-      <c r="AI17">
-        <v>0</v>
-      </c>
-      <c r="AJ17">
-        <v>0</v>
-      </c>
-      <c r="AK17">
-        <v>0</v>
       </c>
       <c r="AL17">
         <v>0</v>
@@ -2714,7 +3478,7 @@
     </row>
     <row r="18" spans="1:41">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2753,10 +3517,10 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -2804,22 +3568,22 @@
         <v>0</v>
       </c>
       <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
         <v>100</v>
-      </c>
-      <c r="AF18">
-        <v>0</v>
       </c>
       <c r="AG18">
         <v>100</v>
       </c>
       <c r="AH18">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AI18">
         <v>0</v>
       </c>
       <c r="AJ18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AK18">
         <v>0</v>
@@ -2839,7 +3603,7 @@
     </row>
     <row r="19" spans="1:41">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2964,7 +3728,7 @@
     </row>
     <row r="20" spans="1:41">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3089,7 +3853,7 @@
     </row>
     <row r="21" spans="1:41">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3214,7 +3978,7 @@
     </row>
     <row r="22" spans="1:41">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3339,7 +4103,7 @@
     </row>
     <row r="23" spans="1:41">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -3348,14 +4112,14 @@
         <v>0</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>0.1137846627281003</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
       <c r="G23">
         <v>0</v>
       </c>
@@ -3369,28 +4133,28 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>0.957305857086254</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <v>0.1137846627281003</v>
       </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
       <c r="Q23">
         <v>0</v>
       </c>
       <c r="R23">
-        <v>0.957305857086254</v>
+        <v>0</v>
       </c>
       <c r="S23">
         <v>0</v>
@@ -3423,48 +4187,48 @@
         <v>0</v>
       </c>
       <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
         <v>0.1137846627281003</v>
       </c>
-      <c r="AD23">
-        <v>0</v>
-      </c>
-      <c r="AE23">
-        <v>0</v>
-      </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
-      <c r="AG23">
-        <v>0</v>
-      </c>
-      <c r="AH23">
-        <v>0</v>
-      </c>
-      <c r="AI23">
-        <v>0</v>
-      </c>
-      <c r="AJ23">
-        <v>0</v>
-      </c>
       <c r="AK23">
         <v>0</v>
       </c>
       <c r="AL23">
-        <v>0</v>
+        <v>0.9553335431483193</v>
       </c>
       <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
         <v>0.1137846627281</v>
-      </c>
-      <c r="AN23">
-        <v>0.9553335431483193</v>
-      </c>
-      <c r="AO23">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:41">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -3473,14 +4237,14 @@
         <v>0</v>
       </c>
       <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>2.558208211429871</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
       <c r="G24">
         <v>0</v>
       </c>
@@ -3494,28 +4258,28 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>21.52300359056355</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
         <v>2.55820821142987</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24">
-        <v>21.52300359056355</v>
+        <v>0</v>
       </c>
       <c r="S24">
         <v>0</v>
@@ -3548,48 +4312,48 @@
         <v>0</v>
       </c>
       <c r="AC24">
+        <v>100</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <v>0</v>
+      </c>
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24">
         <v>2.55820821142987</v>
       </c>
-      <c r="AD24">
-        <v>100</v>
-      </c>
-      <c r="AE24">
-        <v>0</v>
-      </c>
-      <c r="AF24">
-        <v>0</v>
-      </c>
-      <c r="AG24">
-        <v>0</v>
-      </c>
-      <c r="AH24">
-        <v>0</v>
-      </c>
-      <c r="AI24">
-        <v>0</v>
-      </c>
-      <c r="AJ24">
-        <v>0</v>
-      </c>
       <c r="AK24">
         <v>0</v>
       </c>
       <c r="AL24">
-        <v>0</v>
+        <v>21.4786602705539</v>
       </c>
       <c r="AM24">
+        <v>0</v>
+      </c>
+      <c r="AN24">
+        <v>0</v>
+      </c>
+      <c r="AO24">
         <v>2.558208211429879</v>
-      </c>
-      <c r="AN24">
-        <v>21.4786602705539</v>
-      </c>
-      <c r="AO24">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:41">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3714,7 +4478,7 @@
     </row>
     <row r="26" spans="1:41">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3780,10 +4544,10 @@
         <v>0</v>
       </c>
       <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
         <v>100</v>
-      </c>
-      <c r="X26">
-        <v>0</v>
       </c>
       <c r="Y26">
         <v>0</v>
@@ -3842,7 +4606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D2"/>
   <sheetViews>
@@ -3852,16 +4616,16 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3869,7 +4633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E60"/>
   <sheetViews>
@@ -3879,22 +4643,22 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -3903,10 +4667,10 @@
     <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D4">
         <v>4640</v>
@@ -3915,10 +4679,10 @@
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D5">
         <v>65</v>
@@ -3927,10 +4691,10 @@
     <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -3939,10 +4703,10 @@
     <row r="7" spans="1:4">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D7">
         <v>2.379487179487179</v>
@@ -3951,10 +4715,10 @@
     <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D8">
         <v>4539.973846153845</v>
@@ -3963,10 +4727,10 @@
     <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D9">
         <v>13920</v>
@@ -3974,11 +4738,11 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3986,22 +4750,22 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -4010,10 +4774,10 @@
     <row r="15" spans="1:4">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D15">
         <v>11530</v>
@@ -4022,10 +4786,10 @@
     <row r="16" spans="1:4">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D16">
         <v>170</v>
@@ -4034,10 +4798,10 @@
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D17">
         <v>50</v>
@@ -4046,10 +4810,10 @@
     <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D18">
         <v>1.356470588235294</v>
@@ -4058,10 +4822,10 @@
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D19">
         <v>11462.02729411765</v>
@@ -4070,10 +4834,10 @@
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D20">
         <v>23060</v>
@@ -4081,11 +4845,11 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4093,25 +4857,25 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="D25">
         <v>28541.6875</v>
@@ -4122,11 +4886,11 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="D26">
         <v>356.4903214361887</v>
@@ -4134,22 +4898,22 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D30">
         <v>16</v>
@@ -4158,7 +4922,7 @@
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="D31">
         <v>28541.6875</v>
@@ -4167,10 +4931,10 @@
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D32">
         <v>3.5</v>
@@ -4179,10 +4943,10 @@
     <row r="33" spans="1:4">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D33">
         <v>0.06</v>
@@ -4191,10 +4955,10 @@
     <row r="34" spans="1:4">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D34">
         <v>0.02107407617698663</v>
@@ -4203,10 +4967,10 @@
     <row r="35" spans="1:4">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -4215,10 +4979,10 @@
     <row r="36" spans="1:4">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -4227,10 +4991,10 @@
     <row r="37" spans="1:4">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D37">
         <v>5708337.5</v>
@@ -4239,10 +5003,10 @@
     <row r="38" spans="1:4">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D38">
         <v>24694268.025</v>
@@ -4251,10 +5015,10 @@
     <row r="39" spans="1:4">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D39">
         <v>9133340</v>
@@ -4263,10 +5027,10 @@
     <row r="40" spans="1:4">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D40">
         <v>81754809.675</v>
@@ -4275,10 +5039,10 @@
     <row r="41" spans="1:4">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D41">
         <v>71925.05250000001</v>
@@ -4287,10 +5051,10 @@
     <row r="42" spans="1:4">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D42">
         <v>791432.4526874999</v>
@@ -4299,10 +5063,10 @@
     <row r="43" spans="1:4">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D43">
         <v>2113569.04275</v>
@@ -4311,10 +5075,10 @@
     <row r="44" spans="1:4">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D44">
         <v>6336.254625</v>
@@ -4322,13 +5086,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="D45">
         <v>15783553.1875</v>
@@ -4336,11 +5100,11 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="D46">
         <v>180.1775478025114</v>
@@ -4348,22 +5112,22 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="D50">
         <v>19</v>
@@ -4372,10 +5136,10 @@
     <row r="51" spans="1:4">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D51">
         <v>142.8</v>
@@ -4384,7 +5148,7 @@
     <row r="52" spans="1:4">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="D52">
         <v>30</v>
@@ -4393,10 +5157,10 @@
     <row r="53" spans="1:4">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D53">
         <v>130.2</v>
@@ -4405,7 +5169,7 @@
     <row r="54" spans="1:4">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="D54">
         <v>19</v>
@@ -4414,10 +5178,10 @@
     <row r="55" spans="1:4">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D55">
         <v>357</v>
@@ -4426,7 +5190,7 @@
     <row r="56" spans="1:4">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4435,10 +5199,10 @@
     <row r="57" spans="1:4">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D57">
         <v>259.1573099999999</v>
@@ -4447,10 +5211,10 @@
     <row r="58" spans="1:4">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="D58">
         <v>9624.423774272149</v>
@@ -4459,10 +5223,10 @@
     <row r="59" spans="1:4">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D59">
         <v>1463</v>
@@ -4470,11 +5234,11 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="D60">
         <v>0</v>

</xml_diff>